<commit_message>
Update control y errores
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Galrich\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tatiux\Desktop\Fractum2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8232"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="123">
   <si>
     <t>Caso de uso</t>
   </si>
@@ -204,15 +204,9 @@
     <t>View/incidencias/consultarJefe.php</t>
   </si>
   <si>
-    <t>1.4?</t>
-  </si>
-  <si>
     <t>View/incidencias/modificarJefe.php</t>
   </si>
   <si>
-    <t>SIN IMPLEMENTAR</t>
-  </si>
-  <si>
     <t>View/usuarios/altaInternoJefe.php</t>
   </si>
   <si>
@@ -270,9 +264,6 @@
     <t>Detalle</t>
   </si>
   <si>
-    <t>1.3,2.2</t>
-  </si>
-  <si>
     <t>View/incidencias/listarInterno.php</t>
   </si>
   <si>
@@ -394,6 +385,15 @@
   </si>
   <si>
     <t>anotar las variables de sesión en la hoja y acabar con JavaScript</t>
+  </si>
+  <si>
+    <t>View/usuarios/buscarJefe.php</t>
+  </si>
+  <si>
+    <t>View/usuarios/buscarInterno.php</t>
+  </si>
+  <si>
+    <t>View/usuarios/buscarExterno.php</t>
   </si>
 </sst>
 </file>
@@ -801,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -862,59 +862,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -939,6 +888,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1221,127 +1225,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView tabSelected="1" topLeftCell="R8" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.77734375" customWidth="1"/>
-    <col min="18" max="18" width="10.77734375" style="20" customWidth="1"/>
-    <col min="19" max="19" width="15.77734375" customWidth="1"/>
-    <col min="20" max="20" width="10.77734375" style="20" customWidth="1"/>
-    <col min="21" max="21" width="15.77734375" customWidth="1"/>
-    <col min="22" max="22" width="10.77734375" style="20" customWidth="1"/>
-    <col min="24" max="24" width="15.77734375" customWidth="1"/>
-    <col min="26" max="26" width="15.77734375" customWidth="1"/>
-    <col min="28" max="28" width="15.77734375" customWidth="1"/>
+    <col min="13" max="13" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="20" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="20" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="20" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
+    <col min="26" max="26" width="15.7109375" customWidth="1"/>
+    <col min="28" max="28" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+    <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="52"/>
       <c r="C2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="Q2" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="28"/>
-      <c r="X2" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="28"/>
-    </row>
-    <row r="3" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="37" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="Q2" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="40"/>
+      <c r="X2" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="40"/>
+    </row>
+    <row r="3" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="34" t="s">
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="36"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="29" t="s">
+      <c r="Q3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="30"/>
-      <c r="S3" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="T3" s="30"/>
-      <c r="U3" s="29" t="s">
+      <c r="R3" s="42"/>
+      <c r="S3" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="T3" s="42"/>
+      <c r="U3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="30"/>
-      <c r="X3" s="29" t="s">
+      <c r="V3" s="42"/>
+      <c r="X3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="29" t="s">
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA3" s="42"/>
+      <c r="AB3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AC3" s="30"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
+      <c r="AC3" s="42"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>5</v>
@@ -1350,10 +1354,10 @@
         <v>52</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>5</v>
@@ -1362,10 +1366,10 @@
         <v>52</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M4" s="9" t="s">
         <v>5</v>
@@ -1374,52 +1378,52 @@
         <v>52</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="S4" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="T4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="U4" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="V4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="X4" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Y4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="Z4" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AA4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="AB4" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AC4" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="AF4" s="54"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="AF4" s="37"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1" t="s">
         <v>46</v>
@@ -1453,18 +1457,18 @@
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S5" s="21"/>
       <c r="T5" s="23"/>
       <c r="U5" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="V5" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="X5" s="21"/>
       <c r="Y5" s="23"/>
@@ -1473,11 +1477,11 @@
       <c r="AB5" s="21"/>
       <c r="AC5" s="23"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1" t="s">
         <v>46</v>
@@ -1493,17 +1497,17 @@
         <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="3">
-        <v>2.1</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="3"/>
       <c r="L6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="3">
@@ -1511,41 +1515,45 @@
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="S6" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="T6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="U6" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="V6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="X6" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z6" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="R6" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="S6" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="U6" s="21" t="s">
+      <c r="AA6" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB6" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="V6" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="X6" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="21" t="s">
-        <v>118</v>
-      </c>
       <c r="AC6" s="23"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
         <v>46</v>
@@ -1571,10 +1579,10 @@
       <c r="O7" s="3"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R7" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S7" s="21"/>
       <c r="T7" s="23"/>
@@ -1587,11 +1595,11 @@
       <c r="AB7" s="21"/>
       <c r="AC7" s="23"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="2"/>
       <c r="D8" s="1" t="s">
         <v>46</v>
@@ -1599,10 +1607,10 @@
       <c r="E8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3">
-        <v>1.2</v>
-      </c>
+      <c r="F8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1617,29 +1625,31 @@
       <c r="O8" s="3"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R8" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S8" s="21"/>
       <c r="T8" s="23"/>
       <c r="U8" s="21"/>
       <c r="V8" s="23"/>
       <c r="X8" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y8" s="23"/>
+        <v>111</v>
+      </c>
+      <c r="Y8" s="23" t="s">
+        <v>110</v>
+      </c>
       <c r="Z8" s="21"/>
       <c r="AA8" s="23"/>
       <c r="AB8" s="21"/>
       <c r="AC8" s="23"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="32"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
         <v>46</v>
@@ -1647,10 +1657,10 @@
       <c r="E9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3">
-        <v>1.2</v>
-      </c>
+      <c r="F9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1665,29 +1675,31 @@
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S9" s="21"/>
       <c r="T9" s="23"/>
       <c r="U9" s="21"/>
       <c r="V9" s="23"/>
       <c r="X9" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y9" s="23"/>
+        <v>111</v>
+      </c>
+      <c r="Y9" s="23" t="s">
+        <v>110</v>
+      </c>
       <c r="Z9" s="21"/>
       <c r="AA9" s="23"/>
       <c r="AB9" s="21"/>
       <c r="AC9" s="23"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="32"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
         <v>46</v>
@@ -1709,7 +1721,7 @@
         <v>46</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>46</v>
@@ -1717,18 +1729,18 @@
       <c r="O10" s="3"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R10" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S10" s="21"/>
       <c r="T10" s="23"/>
       <c r="U10" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="V10" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="X10" s="21"/>
       <c r="Y10" s="23"/>
@@ -1737,11 +1749,11 @@
       <c r="AB10" s="21"/>
       <c r="AC10" s="23"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="32"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1" t="s">
         <v>46</v>
@@ -1750,66 +1762,70 @@
         <v>55</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
-        <v>57</v>
+      <c r="G11" s="3">
+        <v>1.1000000000000001</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="3" t="s">
-        <v>81</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="3"/>
       <c r="L11" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R11" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S11" s="21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="T11" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="U11" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="V11" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="X11" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y11" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z11" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA11" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB11" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="V11" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="X11" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="21" t="s">
-        <v>118</v>
-      </c>
       <c r="AC11" s="23"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="32"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1" t="s">
         <v>46</v>
@@ -1825,17 +1841,17 @@
         <v>46</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="3">
-        <v>2.2999999999999998</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="3"/>
       <c r="L12" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>46</v>
@@ -1843,37 +1859,39 @@
       <c r="O12" s="3"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S12" s="21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="T12" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="U12" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="V12" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="X12" s="21"/>
       <c r="Y12" s="23"/>
       <c r="Z12" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA12" s="23"/>
+        <v>114</v>
+      </c>
+      <c r="AA12" s="23" t="s">
+        <v>110</v>
+      </c>
       <c r="AB12" s="21"/>
       <c r="AC12" s="23"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="32"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="2"/>
       <c r="D13" s="1" t="s">
         <v>46</v>
@@ -1881,15 +1899,15 @@
       <c r="E13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="F13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="3"/>
       <c r="H13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>46</v>
@@ -1899,7 +1917,7 @@
         <v>46</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>46</v>
@@ -1907,45 +1925,47 @@
       <c r="O13" s="3"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S13" s="21"/>
       <c r="T13" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="U13" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="V13" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="X13" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y13" s="23"/>
+        <v>111</v>
+      </c>
+      <c r="Y13" s="23" t="s">
+        <v>110</v>
+      </c>
       <c r="Z13" s="21"/>
       <c r="AA13" s="23"/>
       <c r="AB13" s="21"/>
       <c r="AC13" s="23"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="32"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="3">
-        <v>1.5</v>
+      <c r="G14" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>49</v>
@@ -1961,82 +1981,106 @@
       <c r="O14" s="3"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S14" s="21"/>
       <c r="T14" s="23"/>
       <c r="U14" s="21"/>
       <c r="V14" s="23"/>
       <c r="X14" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y14" s="23"/>
+        <v>111</v>
+      </c>
+      <c r="Y14" s="23" t="s">
+        <v>108</v>
+      </c>
       <c r="Z14" s="21"/>
       <c r="AA14" s="23"/>
       <c r="AB14" s="21"/>
       <c r="AC14" s="23"/>
     </row>
-    <row r="15" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>120</v>
+      </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="2"/>
+      <c r="G15" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>121</v>
+      </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="2"/>
+      <c r="K15" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>122</v>
+      </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="3"/>
+      <c r="O15" s="3">
+        <v>4.0999999999999996</v>
+      </c>
       <c r="P15" s="4"/>
-      <c r="Q15" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="R15" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="S15" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="T15" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="U15" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="V15" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="X15" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y15" s="45"/>
-      <c r="Z15" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA15" s="45"/>
-      <c r="AB15" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC15" s="45"/>
-    </row>
-    <row r="16" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="32" t="s">
+      <c r="Q15" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="R15" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S15" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="T15" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="U15" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="V15" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="X15" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y15" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z15" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA15" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB15" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC15" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="14"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -2050,30 +2094,30 @@
       <c r="N16" s="10"/>
       <c r="O16" s="16"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="49"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="49"/>
-      <c r="T16" s="48"/>
-      <c r="U16" s="49"/>
-      <c r="V16" s="48"/>
-      <c r="X16" s="49"/>
-      <c r="Y16" s="48"/>
-      <c r="Z16" s="49"/>
-      <c r="AA16" s="48"/>
-      <c r="AB16" s="49"/>
-      <c r="AC16" s="48"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="Q16" s="32"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="31"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="32"/>
+      <c r="AC16" s="31"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="43"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>46</v>
@@ -2092,32 +2136,32 @@
       <c r="N17" s="2"/>
       <c r="O17" s="3"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="R17" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="S17" s="46"/>
-      <c r="T17" s="47"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="47"/>
-      <c r="X17" s="46"/>
-      <c r="Y17" s="47"/>
-      <c r="Z17" s="46"/>
-      <c r="AA17" s="47"/>
-      <c r="AB17" s="46"/>
-      <c r="AC17" s="47"/>
-    </row>
-    <row r="18" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
+      <c r="Q17" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="R17" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="S17" s="29"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="30"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="30"/>
+    </row>
+    <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="2"/>
       <c r="D18" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>46</v>
@@ -2136,28 +2180,28 @@
       <c r="N18" s="2"/>
       <c r="O18" s="3"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="R18" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="S18" s="44"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="44"/>
-      <c r="V18" s="45"/>
-      <c r="X18" s="44"/>
-      <c r="Y18" s="45"/>
-      <c r="Z18" s="44"/>
-      <c r="AA18" s="45"/>
-      <c r="AB18" s="44"/>
-      <c r="AC18" s="45"/>
-    </row>
-    <row r="19" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="Q18" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R18" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="S18" s="27"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="28"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="27"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="27"/>
+      <c r="AC18" s="28"/>
+    </row>
+    <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="33"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
@@ -2178,30 +2222,30 @@
       <c r="N19" s="2"/>
       <c r="O19" s="3"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="48"/>
-      <c r="S19" s="49"/>
-      <c r="T19" s="48"/>
-      <c r="U19" s="49"/>
-      <c r="V19" s="48"/>
-      <c r="X19" s="49"/>
-      <c r="Y19" s="48"/>
-      <c r="Z19" s="49"/>
-      <c r="AA19" s="48"/>
-      <c r="AB19" s="49"/>
-      <c r="AC19" s="48"/>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
+      <c r="Q19" s="32"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="31"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="32"/>
+      <c r="AA19" s="31"/>
+      <c r="AB19" s="32"/>
+      <c r="AC19" s="31"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>46</v>
@@ -2211,7 +2255,7 @@
         <v>46</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>46</v>
@@ -2221,47 +2265,47 @@
         <v>46</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="R20" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="S20" s="46"/>
-      <c r="T20" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="U20" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="V20" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="X20" s="46"/>
-      <c r="Y20" s="47"/>
-      <c r="Z20" s="46"/>
-      <c r="AA20" s="47"/>
-      <c r="AB20" s="46"/>
-      <c r="AC20" s="47"/>
-    </row>
-    <row r="21" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
+      <c r="Q20" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="R20" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="S20" s="29"/>
+      <c r="T20" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="U20" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="V20" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="30"/>
+      <c r="AB20" s="29"/>
+      <c r="AC20" s="30"/>
+    </row>
+    <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="33"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>46</v>
@@ -2271,7 +2315,7 @@
         <v>46</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>46</v>
@@ -2281,42 +2325,42 @@
         <v>46</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>46</v>
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="R21" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="S21" s="44"/>
-      <c r="T21" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="U21" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="V21" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="X21" s="44"/>
-      <c r="Y21" s="45"/>
-      <c r="Z21" s="44"/>
-      <c r="AA21" s="45"/>
-      <c r="AB21" s="44"/>
-      <c r="AC21" s="45"/>
-    </row>
-    <row r="22" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="32" t="s">
+      <c r="Q21" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R21" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="S21" s="27"/>
+      <c r="T21" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="U21" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="V21" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="27"/>
+      <c r="AC21" s="28"/>
+    </row>
+    <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="14"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -2330,45 +2374,45 @@
       <c r="N22" s="2"/>
       <c r="O22" s="3"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="48"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="48"/>
-      <c r="U22" s="49"/>
-      <c r="V22" s="48"/>
-      <c r="X22" s="49"/>
-      <c r="Y22" s="48"/>
-      <c r="Z22" s="49"/>
-      <c r="AA22" s="48"/>
-      <c r="AB22" s="49"/>
-      <c r="AC22" s="48"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
+      <c r="Q22" s="32"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="31"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="32"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="32"/>
+      <c r="AC22" s="31"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="43"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="3">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="3">
-        <v>1.3</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K23" s="3"/>
       <c r="L23" s="1" t="s">
         <v>49</v>
       </c>
@@ -2376,54 +2420,58 @@
       <c r="N23" s="2"/>
       <c r="O23" s="3"/>
       <c r="P23" s="4"/>
-      <c r="Q23" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="R23" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="S23" s="46"/>
-      <c r="T23" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="U23" s="46"/>
-      <c r="V23" s="47"/>
-      <c r="X23" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y23" s="47"/>
-      <c r="Z23" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA23" s="47"/>
-      <c r="AB23" s="46"/>
-      <c r="AC23" s="47"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+      <c r="Q23" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="R23" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="S23" s="29"/>
+      <c r="T23" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="U23" s="29"/>
+      <c r="V23" s="30"/>
+      <c r="X23" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y23" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z23" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA23" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB23" s="29"/>
+      <c r="AC23" s="30"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="33"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="2"/>
       <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="19">
-        <v>1.7</v>
+      <c r="G24" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J24" s="2"/>
-      <c r="K24" s="3">
-        <v>2.5</v>
+      <c r="K24" s="19">
+        <v>2.1</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>49</v>
@@ -2433,33 +2481,35 @@
       <c r="O24" s="19"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R24" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S24" s="21"/>
       <c r="T24" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="23"/>
       <c r="X24" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Y24" s="23"/>
       <c r="Z24" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA24" s="23"/>
+        <v>107</v>
+      </c>
+      <c r="AA24" s="23" t="s">
+        <v>108</v>
+      </c>
       <c r="AB24" s="21"/>
       <c r="AC24" s="23"/>
     </row>
-    <row r="25" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="33"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="2"/>
       <c r="D25" s="1" t="s">
         <v>46</v>
@@ -2475,58 +2525,60 @@
         <v>46</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J25" s="2"/>
-      <c r="K25" s="3">
-        <v>2.4</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" s="3"/>
       <c r="L25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="3">
         <v>3.4</v>
       </c>
       <c r="P25" s="4"/>
-      <c r="Q25" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="R25" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="S25" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="T25" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="U25" s="44" t="s">
+      <c r="Q25" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R25" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="S25" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="T25" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="U25" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="V25" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="28"/>
+      <c r="Z25" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA25" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB25" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="V25" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="X25" s="44"/>
-      <c r="Y25" s="45"/>
-      <c r="Z25" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA25" s="45"/>
-      <c r="AB25" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC25" s="45"/>
-    </row>
-    <row r="26" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="32" t="s">
+      <c r="AC25" s="28"/>
+    </row>
+    <row r="26" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="14"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2540,24 +2592,24 @@
       <c r="N26" s="2"/>
       <c r="O26" s="3"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="48"/>
-      <c r="S26" s="49"/>
-      <c r="T26" s="48"/>
-      <c r="U26" s="49"/>
-      <c r="V26" s="48"/>
-      <c r="X26" s="49"/>
-      <c r="Y26" s="48"/>
-      <c r="Z26" s="49"/>
-      <c r="AA26" s="48"/>
-      <c r="AB26" s="49"/>
-      <c r="AC26" s="48"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
+      <c r="Q26" s="32"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="32"/>
+      <c r="V26" s="31"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="32"/>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="32"/>
+      <c r="AC26" s="31"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A27" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="33"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1" t="s">
         <v>49</v>
@@ -2569,77 +2621,77 @@
         <v>46</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="3">
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="3">
         <v>3.5</v>
       </c>
       <c r="P27" s="4"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="47"/>
-      <c r="S27" s="46"/>
-      <c r="T27" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="U27" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="V27" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="X27" s="46"/>
-      <c r="Y27" s="47"/>
-      <c r="Z27" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA27" s="47"/>
-      <c r="AB27" s="46" t="s">
+      <c r="Q27" s="29"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="U27" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="AC27" s="47"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A28" s="33" t="s">
+      <c r="V27" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA27" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB27" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC27" s="30"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="33"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="3">
-        <v>1.8</v>
-      </c>
+      <c r="G28" s="3"/>
       <c r="H28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J28" s="2"/>
-      <c r="K28" s="3">
-        <v>1.8</v>
+      <c r="K28" s="19">
+        <v>2.2999999999999998</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="3">
@@ -2647,45 +2699,45 @@
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R28" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S28" s="21"/>
       <c r="T28" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="U28" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="V28" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="X28" s="21" t="s">
-        <v>114</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="X28" s="21"/>
       <c r="Y28" s="23"/>
       <c r="Z28" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA28" s="23"/>
+        <v>107</v>
+      </c>
+      <c r="AA28" s="23" t="s">
+        <v>108</v>
+      </c>
       <c r="AB28" s="21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AC28" s="23"/>
     </row>
-    <row r="29" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="33" t="s">
+    <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="33"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>46</v>
@@ -2695,7 +2747,7 @@
         <v>46</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>46</v>
@@ -2705,44 +2757,44 @@
         <v>46</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="3">
         <v>3.6</v>
       </c>
       <c r="P29" s="4"/>
-      <c r="Q29" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="R29" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="S29" s="44"/>
-      <c r="T29" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="U29" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="V29" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="X29" s="44"/>
-      <c r="Y29" s="45"/>
-      <c r="Z29" s="44"/>
-      <c r="AA29" s="45"/>
-      <c r="AB29" s="44" t="s">
+      <c r="Q29" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R29" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="S29" s="27"/>
+      <c r="T29" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="U29" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="AC29" s="45"/>
-    </row>
-    <row r="30" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="32" t="s">
+      <c r="V29" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="28"/>
+      <c r="Z29" s="27"/>
+      <c r="AA29" s="28"/>
+      <c r="AB29" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC29" s="28"/>
+    </row>
+    <row r="30" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="14"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -2756,31 +2808,31 @@
       <c r="N30" s="2"/>
       <c r="O30" s="3"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="48"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="48"/>
-      <c r="U30" s="49"/>
-      <c r="V30" s="48"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="31"/>
       <c r="W30" s="4"/>
-      <c r="X30" s="49"/>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="49"/>
-      <c r="AA30" s="48"/>
-      <c r="AB30" s="49"/>
-      <c r="AC30" s="48"/>
-    </row>
-    <row r="31" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="33" t="s">
+      <c r="X30" s="32"/>
+      <c r="Y30" s="31"/>
+      <c r="Z30" s="32"/>
+      <c r="AA30" s="31"/>
+      <c r="AB30" s="32"/>
+      <c r="AC30" s="31"/>
+    </row>
+    <row r="31" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="33"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="2"/>
       <c r="D31" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>46</v>
@@ -2799,24 +2851,24 @@
       <c r="N31" s="2"/>
       <c r="O31" s="3"/>
       <c r="P31" s="4"/>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="53"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="53"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="53"/>
-      <c r="X31" s="52"/>
-      <c r="Y31" s="53"/>
-      <c r="Z31" s="52"/>
-      <c r="AA31" s="53"/>
-      <c r="AB31" s="52"/>
-      <c r="AC31" s="53"/>
-    </row>
-    <row r="32" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="33" t="s">
+      <c r="Q31" s="35"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="35"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="35"/>
+      <c r="V31" s="36"/>
+      <c r="X31" s="35"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="35"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="35"/>
+      <c r="AC31" s="36"/>
+    </row>
+    <row r="32" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="43"/>
       <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
@@ -2837,35 +2889,35 @@
       <c r="N32" s="2"/>
       <c r="O32" s="3"/>
       <c r="P32" s="4"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="48"/>
-      <c r="S32" s="49"/>
-      <c r="T32" s="48"/>
-      <c r="U32" s="49"/>
-      <c r="V32" s="48"/>
-      <c r="X32" s="49"/>
-      <c r="Y32" s="48"/>
-      <c r="Z32" s="49"/>
-      <c r="AA32" s="48"/>
-      <c r="AB32" s="49"/>
-      <c r="AC32" s="48"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
+      <c r="Q32" s="32"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="31"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="31"/>
+      <c r="Z32" s="32"/>
+      <c r="AA32" s="31"/>
+      <c r="AB32" s="32"/>
+      <c r="AC32" s="31"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A33" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="33"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="2"/>
       <c r="D33" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="3">
-        <v>1.9</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="3"/>
       <c r="H33" s="1" t="s">
         <v>49</v>
       </c>
@@ -2879,46 +2931,46 @@
       <c r="N33" s="2"/>
       <c r="O33" s="3"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="R33" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="S33" s="46"/>
-      <c r="T33" s="47"/>
-      <c r="U33" s="46"/>
-      <c r="V33" s="47"/>
-      <c r="X33" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y33" s="47"/>
-      <c r="Z33" s="46"/>
-      <c r="AA33" s="47"/>
-      <c r="AB33" s="46"/>
-      <c r="AC33" s="47"/>
-    </row>
-    <row r="34" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="33" t="s">
+      <c r="Q33" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="R33" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="S33" s="29"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="29"/>
+      <c r="V33" s="30"/>
+      <c r="X33" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y33" s="30"/>
+      <c r="Z33" s="29"/>
+      <c r="AA33" s="30"/>
+      <c r="AB33" s="29"/>
+      <c r="AC33" s="30"/>
+    </row>
+    <row r="34" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="33"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="2"/>
       <c r="D34" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="3">
-        <v>1.9</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="3"/>
       <c r="H34" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>46</v>
@@ -2928,46 +2980,48 @@
         <v>46</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>46</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="4"/>
-      <c r="Q34" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="R34" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="S34" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="T34" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="U34" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="V34" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="X34" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y34" s="45"/>
-      <c r="Z34" s="44"/>
-      <c r="AA34" s="45"/>
-      <c r="AB34" s="44"/>
-      <c r="AC34" s="45"/>
-    </row>
-    <row r="35" spans="1:29" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="32" t="s">
+      <c r="Q34" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R34" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S34" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="T34" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="U34" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="V34" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="X34" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y34" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z34" s="27"/>
+      <c r="AA34" s="28"/>
+      <c r="AB34" s="27"/>
+      <c r="AC34" s="28"/>
+    </row>
+    <row r="35" spans="1:29" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="14"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -2981,30 +3035,30 @@
       <c r="N35" s="9"/>
       <c r="O35" s="15"/>
       <c r="P35" s="18"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="51"/>
-      <c r="T35" s="50"/>
-      <c r="U35" s="49"/>
-      <c r="V35" s="50"/>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="50"/>
-      <c r="Z35" s="51"/>
-      <c r="AA35" s="50"/>
-      <c r="AB35" s="49"/>
-      <c r="AC35" s="50"/>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A36" s="33" t="s">
+      <c r="Q35" s="32"/>
+      <c r="R35" s="33"/>
+      <c r="S35" s="34"/>
+      <c r="T35" s="33"/>
+      <c r="U35" s="32"/>
+      <c r="V35" s="33"/>
+      <c r="X35" s="32"/>
+      <c r="Y35" s="33"/>
+      <c r="Z35" s="34"/>
+      <c r="AA35" s="33"/>
+      <c r="AB35" s="32"/>
+      <c r="AC35" s="33"/>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="33"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="2"/>
       <c r="D36" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>46</v>
@@ -3023,28 +3077,28 @@
       <c r="N36" s="2"/>
       <c r="O36" s="3"/>
       <c r="P36" s="4"/>
-      <c r="Q36" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="R36" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="S36" s="46"/>
-      <c r="T36" s="47"/>
-      <c r="U36" s="46"/>
-      <c r="V36" s="47"/>
-      <c r="X36" s="46"/>
-      <c r="Y36" s="47"/>
-      <c r="Z36" s="46"/>
-      <c r="AA36" s="47"/>
-      <c r="AB36" s="46"/>
-      <c r="AC36" s="47"/>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A37" s="33" t="s">
+      <c r="Q36" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="R36" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="S36" s="29"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="29"/>
+      <c r="V36" s="30"/>
+      <c r="X36" s="29"/>
+      <c r="Y36" s="30"/>
+      <c r="Z36" s="29"/>
+      <c r="AA36" s="30"/>
+      <c r="AB36" s="29"/>
+      <c r="AC36" s="30"/>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="33"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="2"/>
       <c r="D37" s="1" t="s">
         <v>46</v>
@@ -3068,10 +3122,10 @@
       <c r="O37" s="3"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R37" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S37" s="21"/>
       <c r="T37" s="23"/>
@@ -3084,22 +3138,22 @@
       <c r="AB37" s="21"/>
       <c r="AC37" s="23"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A38" s="33" t="s">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A38" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="33"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="2"/>
       <c r="D38" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="3">
-        <v>1.1000000000000001</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="3"/>
       <c r="H38" s="1" t="s">
         <v>49</v>
       </c>
@@ -3114,40 +3168,42 @@
       <c r="O38" s="3"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R38" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S38" s="21"/>
       <c r="T38" s="23"/>
       <c r="U38" s="21"/>
       <c r="V38" s="23"/>
       <c r="X38" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y38" s="23"/>
+        <v>111</v>
+      </c>
+      <c r="Y38" s="23" t="s">
+        <v>110</v>
+      </c>
       <c r="Z38" s="21"/>
       <c r="AA38" s="23"/>
       <c r="AB38" s="21"/>
       <c r="AC38" s="23"/>
     </row>
-    <row r="39" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="33" t="s">
+    <row r="39" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="33"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="2"/>
       <c r="D39" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="3">
-        <v>1.1100000000000001</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="3"/>
       <c r="H39" s="1" t="s">
         <v>49</v>
       </c>
@@ -3158,44 +3214,48 @@
         <v>46</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="3">
-        <v>3.7</v>
+        <v>3.1</v>
       </c>
       <c r="P39" s="4"/>
-      <c r="Q39" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="R39" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="S39" s="44"/>
-      <c r="T39" s="45"/>
-      <c r="U39" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="V39" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="X39" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y39" s="45"/>
-      <c r="Z39" s="44"/>
-      <c r="AA39" s="45"/>
-      <c r="AB39" s="44" t="s">
+      <c r="Q39" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R39" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S39" s="27"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="AC39" s="45"/>
-    </row>
-    <row r="40" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="32" t="s">
+      <c r="V39" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="X39" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y39" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z39" s="27"/>
+      <c r="AA39" s="28"/>
+      <c r="AB39" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC39" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="14"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -3209,30 +3269,30 @@
       <c r="N40" s="2"/>
       <c r="O40" s="3"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="49"/>
-      <c r="R40" s="48"/>
-      <c r="S40" s="49"/>
-      <c r="T40" s="48"/>
-      <c r="U40" s="49"/>
-      <c r="V40" s="48"/>
-      <c r="X40" s="49"/>
-      <c r="Y40" s="48"/>
-      <c r="Z40" s="49"/>
-      <c r="AA40" s="48"/>
-      <c r="AB40" s="49"/>
-      <c r="AC40" s="48"/>
-    </row>
-    <row r="41" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="33" t="s">
+      <c r="Q40" s="32"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="32"/>
+      <c r="V40" s="31"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="32"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="31"/>
+    </row>
+    <row r="41" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="33"/>
+      <c r="B41" s="43"/>
       <c r="C41" s="2"/>
       <c r="D41" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>46</v>
@@ -3251,28 +3311,28 @@
       <c r="N41" s="2"/>
       <c r="O41" s="3"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="52" t="s">
-        <v>114</v>
-      </c>
-      <c r="R41" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="S41" s="52"/>
-      <c r="T41" s="53"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="53"/>
-      <c r="X41" s="52"/>
-      <c r="Y41" s="53"/>
-      <c r="Z41" s="52"/>
-      <c r="AA41" s="53"/>
-      <c r="AB41" s="52"/>
-      <c r="AC41" s="53"/>
-    </row>
-    <row r="42" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="33" t="s">
+      <c r="Q41" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="R41" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="S41" s="35"/>
+      <c r="T41" s="36"/>
+      <c r="U41" s="35"/>
+      <c r="V41" s="36"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="36"/>
+      <c r="Z41" s="35"/>
+      <c r="AA41" s="36"/>
+      <c r="AB41" s="35"/>
+      <c r="AC41" s="36"/>
+    </row>
+    <row r="42" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="33"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="2" t="s">
         <v>50</v>
       </c>
@@ -3295,28 +3355,28 @@
       <c r="N42" s="2"/>
       <c r="O42" s="3"/>
       <c r="P42" s="4"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="48"/>
-      <c r="S42" s="49"/>
-      <c r="T42" s="48"/>
-      <c r="U42" s="49"/>
-      <c r="V42" s="48"/>
-      <c r="X42" s="49"/>
-      <c r="Y42" s="48"/>
-      <c r="Z42" s="49"/>
-      <c r="AA42" s="48"/>
-      <c r="AB42" s="49"/>
-      <c r="AC42" s="48"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A43" s="33" t="s">
+      <c r="Q42" s="32"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="31"/>
+      <c r="U42" s="32"/>
+      <c r="V42" s="31"/>
+      <c r="X42" s="32"/>
+      <c r="Y42" s="31"/>
+      <c r="Z42" s="32"/>
+      <c r="AA42" s="31"/>
+      <c r="AB42" s="32"/>
+      <c r="AC42" s="31"/>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A43" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="33"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="2"/>
       <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>46</v>
@@ -3335,34 +3395,34 @@
       <c r="N43" s="2"/>
       <c r="O43" s="3"/>
       <c r="P43" s="4"/>
-      <c r="Q43" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="R43" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="S43" s="46"/>
-      <c r="T43" s="47"/>
-      <c r="U43" s="46"/>
-      <c r="V43" s="47"/>
-      <c r="X43" s="46"/>
-      <c r="Y43" s="47"/>
-      <c r="Z43" s="46"/>
-      <c r="AA43" s="47"/>
-      <c r="AB43" s="46"/>
-      <c r="AC43" s="47"/>
-    </row>
-    <row r="44" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="33" t="s">
+      <c r="Q43" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="R43" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="S43" s="29"/>
+      <c r="T43" s="30"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="30"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="30"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="30"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="30"/>
+    </row>
+    <row r="44" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="33"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="2"/>
       <c r="D44" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>46</v>
@@ -3382,10 +3442,10 @@
       <c r="O44" s="7"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R44" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S44" s="22"/>
       <c r="T44" s="24"/>
@@ -3398,25 +3458,63 @@
       <c r="AB44" s="22"/>
       <c r="AC44" s="24"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D45" s="13"/>
       <c r="U45" s="4"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="X46" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Y46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="X47" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="Q2:V2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:O2"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A29:B29"/>
     <mergeCell ref="X2:AC2"/>
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="Z3:AA3"/>
@@ -3433,44 +3531,6 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="Q2:V2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E2:O2"/>
-    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3485,11 +3545,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>